<commit_message>
Excel update, new 1Dobservation script
</commit_message>
<xml_diff>
--- a/contrib/Arcadis/Scripts TKI Hydrolib.xlsx
+++ b/contrib/Arcadis/Scripts TKI Hydrolib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scripts\HYDROLIB\contrib\Arcadis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E5F382-855A-4929-B45B-93582C31C8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BBBCA5-AA43-4A69-94DD-ED34F3ED9C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{594B4BF8-64B3-4A35-81CA-455688CA4209}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{594B4BF8-64B3-4A35-81CA-455688CA4209}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     kunstwerken,obseratiepunten en observatieprofielen</t>
       </text>
     </comment>
-    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{9725DA53-9158-46FD-A493-A521E42F02C0}">
+    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{9725DA53-9158-46FD-A493-A521E42F02C0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +63,7 @@
     verschillende modules online zetten, de verschillende blokken</t>
       </text>
     </comment>
-    <comment ref="B8" authorId="2" shapeId="0" xr:uid="{97B35DA6-DE80-4A8B-822C-56B6D2E6E629}">
+    <comment ref="B9" authorId="2" shapeId="0" xr:uid="{97B35DA6-DE80-4A8B-822C-56B6D2E6E629}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -71,7 +71,7 @@
     Uitlezen map/his, statistiek en wegschrijven naar shapefile</t>
       </text>
     </comment>
-    <comment ref="B9" authorId="3" shapeId="0" xr:uid="{021A4381-9F88-491F-9107-C59F3E215AF7}">
+    <comment ref="B10" authorId="3" shapeId="0" xr:uid="{021A4381-9F88-491F-9107-C59F3E215AF7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
   <si>
     <t>Initiele waterstanden obv peilgebieden</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Waterbalans opstellen van deel van de schematisatie</t>
   </si>
   <si>
-    <t>Watergangen verschillende weerstanden geven (o.b.v. shape en waterbreedte)</t>
-  </si>
-  <si>
     <t>1D profielen uitbreiden obv ahn</t>
   </si>
   <si>
@@ -326,9 +323,6 @@
     <t>Stochastentool</t>
   </si>
   <si>
-    <t>Uitlezen lijnen (initiele waterstanden, ruwheden) van GIS naar D-Hydro</t>
-  </si>
-  <si>
     <t>Watergangen verschillende weerstanden obv dwarsprofielen (natuurvriendelijke oevers)</t>
   </si>
   <si>
@@ -357,6 +351,15 @@
   </si>
   <si>
     <t>Measurement locations toevoegen per afwateringseenheid</t>
+  </si>
+  <si>
+    <t>Wegschrijven van ruwheden vanuit GIS (alles overschrijven)</t>
+  </si>
+  <si>
+    <t>Initiele waterstanden obv peilgebieden met behoud van oorspronkelijke waardes</t>
+  </si>
+  <si>
+    <t>Wegschrijven van ruwheden met behoud van oorspronkelijke waardes (o.b.v. shape en waterbreedte)</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,12 +423,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -613,12 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -945,19 +936,19 @@
   <threadedComment ref="B3" dT="2022-03-24T14:59:01.25" personId="{4D9B4A24-E35D-4629-AC6A-DC70F01C9D79}" id="{7172FF8F-699B-4F36-82DC-7524345B38F6}">
     <text>kunstwerken,obseratiepunten en observatieprofielen</text>
   </threadedComment>
-  <threadedComment ref="B7" dT="2022-03-24T14:53:03.20" personId="{4D9B4A24-E35D-4629-AC6A-DC70F01C9D79}" id="{9725DA53-9158-46FD-A493-A521E42F02C0}">
+  <threadedComment ref="B8" dT="2022-03-24T14:53:03.20" personId="{4D9B4A24-E35D-4629-AC6A-DC70F01C9D79}" id="{9725DA53-9158-46FD-A493-A521E42F02C0}">
     <text>lijnen bestanden versimpelen/verfijnen 
 hoogte bepalen voor elke vertex
 gdf naar naar fixed weirs .pli
 .pli bestand inladen om bestaande fixed weirs in te laden om daarna te kunnen wijzigen</text>
   </threadedComment>
-  <threadedComment ref="B7" dT="2022-05-06T09:25:57.80" personId="{2AF68C1F-9613-42B2-8568-F18E48538F28}" id="{44F0C4BA-A7D8-4BD1-A3B8-86A609F96861}" parentId="{9725DA53-9158-46FD-A493-A521E42F02C0}">
+  <threadedComment ref="B8" dT="2022-05-06T09:25:57.80" personId="{2AF68C1F-9613-42B2-8568-F18E48538F28}" id="{44F0C4BA-A7D8-4BD1-A3B8-86A609F96861}" parentId="{9725DA53-9158-46FD-A493-A521E42F02C0}">
     <text>verschillende modules online zetten, de verschillende blokken</text>
   </threadedComment>
-  <threadedComment ref="B8" dT="2022-05-06T09:27:12.41" personId="{2AF68C1F-9613-42B2-8568-F18E48538F28}" id="{97B35DA6-DE80-4A8B-822C-56B6D2E6E629}">
+  <threadedComment ref="B9" dT="2022-05-06T09:27:12.41" personId="{2AF68C1F-9613-42B2-8568-F18E48538F28}" id="{97B35DA6-DE80-4A8B-822C-56B6D2E6E629}">
     <text>Uitlezen map/his, statistiek en wegschrijven naar shapefile</text>
   </threadedComment>
-  <threadedComment ref="B9" dT="2022-05-06T09:41:15.47" personId="{2AF68C1F-9613-42B2-8568-F18E48538F28}" id="{021A4381-9F88-491F-9107-C59F3E215AF7}">
+  <threadedComment ref="B10" dT="2022-05-06T09:41:15.47" personId="{2AF68C1F-9613-42B2-8568-F18E48538F28}" id="{021A4381-9F88-491F-9107-C59F3E215AF7}">
     <text>Als er ruwheden in staan die als basis gebruiken</text>
   </threadedComment>
 </ThreadedComments>
@@ -965,117 +956,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E013BE6A-961E-45DA-8F40-372F6581D9A8}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="76.109375" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
     <col min="8" max="8" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>68</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="9">
         <v>1</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="27"/>
+      <c r="B4" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="26"/>
       <c r="F4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="9">
         <v>1</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>31</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="27"/>
+      <c r="B5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="26"/>
       <c r="F5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
@@ -1084,7 +1075,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1093,367 +1084,361 @@
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="9">
         <v>2</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="9">
-        <v>2</v>
-      </c>
-      <c r="H7" s="32"/>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>71</v>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8" s="9">
         <v>2</v>
       </c>
       <c r="H8" s="32"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="27"/>
+        <v>70</v>
+      </c>
+      <c r="E9" s="26"/>
       <c r="F9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="9">
-        <v>4</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="H9" s="32"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="9">
         <v>4</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G11" s="9">
         <v>4</v>
       </c>
-      <c r="H11" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H11" s="20"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="9">
         <v>4</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="23" t="s">
+        <v>15</v>
+      </c>
       <c r="I12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>32</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
+        <v>14</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="26"/>
       <c r="F13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="9">
         <v>4</v>
       </c>
       <c r="H13" s="23"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>15</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="27"/>
+        <v>32</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" s="9">
         <v>4</v>
       </c>
-      <c r="H14" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>16</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="27"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="26"/>
       <c r="F15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="9">
-        <v>5</v>
-      </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16" s="9">
         <v>5</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>73</v>
+        <v>9</v>
+      </c>
+      <c r="G17" s="9">
+        <v>5</v>
       </c>
       <c r="H17" s="20"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>34</v>
+      </c>
       <c r="B18" s="15" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="27"/>
+      <c r="D18" s="27" t="s">
+        <v>82</v>
+      </c>
       <c r="E18" s="27"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="9"/>
+      <c r="F18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="H18" s="20"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>30</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>73</v>
-      </c>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="20"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
       <c r="F20" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>31</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="20"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>8</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="23"/>
-      <c r="I21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>9</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>44</v>
@@ -1465,78 +1450,79 @@
         <v>10</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="23"/>
       <c r="I22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" s="30" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>46</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
       <c r="F23" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>18</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="9">
-        <v>6</v>
-      </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="10">
+        <v>9</v>
+      </c>
+      <c r="G25" s="9">
         <v>6</v>
       </c>
-      <c r="H25" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H25" s="20"/>
+      <c r="I25" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>8</v>
@@ -1545,76 +1531,78 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G26" s="10">
         <v>6</v>
       </c>
-      <c r="H26" s="33"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H26" s="33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G27" s="10">
         <v>6</v>
       </c>
       <c r="H27" s="33"/>
-      <c r="I27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G28" s="10">
-        <v>8</v>
-      </c>
-      <c r="H28" s="23"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H28" s="33"/>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G29" s="10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" s="23"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1622,121 +1610,118 @@
       <c r="F30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="10">
         <v>9</v>
       </c>
       <c r="H30" s="23"/>
-      <c r="I30" t="s">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="28">
-        <v>22</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>1</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="29"/>
-      <c r="I31" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="G31" s="9">
+        <v>9</v>
+      </c>
+      <c r="H31" s="23"/>
+      <c r="I31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="28">
+        <v>22</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="H32" s="29"/>
+      <c r="I32" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="21"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="H34" s="21"/>
-      <c r="I34" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="21"/>
+      <c r="I35" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>11</v>
       </c>
-      <c r="G35" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="21"/>
-      <c r="I35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>12</v>
-      </c>
       <c r="B36" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1745,145 +1730,166 @@
         <v>10</v>
       </c>
       <c r="G36" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="21"/>
+      <c r="I36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="23"/>
+      <c r="I37" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>29</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="23"/>
-      <c r="I36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>29</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="17" t="s">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="10" t="s">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I40" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I39" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I40" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I41" s="16" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I41" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="19">
+        <v>1</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="19">
-        <v>1</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="19"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="19">
+      <c r="C44" s="19"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="19">
         <v>2</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="19"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="19">
+      <c r="B45" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="19"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="19">
         <v>3</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="19"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="19">
+      <c r="B46" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="19"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="19">
         <v>4</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B47" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="19"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="19">
+        <v>5</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="19"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="19">
-        <v>5</v>
-      </c>
-      <c r="B47" s="19" t="s">
+      <c r="C48" s="19"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="19">
+        <v>6</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="19"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="19">
-        <v>6</v>
-      </c>
-      <c r="B48" s="19" t="s">
+      <c r="C49" s="19"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="19"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>7</v>
-      </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>8</v>
-      </c>
-      <c r="B50" t="s">
-        <v>79</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:G37">
-    <sortCondition ref="G6:G37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:G38">
+    <sortCondition ref="G6:G38"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="H3:H9"/>
+    <mergeCell ref="H26:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>